<commit_message>
update: add missing type and services for chief selection and member entries
</commit_message>
<xml_diff>
--- a/src/assets/DangKyDanhSach.xlsx
+++ b/src/assets/DangKyDanhSach.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA2\SmashHub-FE\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF628F5-036B-4214-868F-8B3D6ED2963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DF6ECD-C122-4A09-87D8-BF91D7E9BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Danh sách thành viên" sheetId="2" r:id="rId1"/>
+    <sheet name="Danh sách đội" sheetId="3" r:id="rId1"/>
+    <sheet name="Danh sách thành viên" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>STT</t>
   </si>
@@ -44,7 +45,13 @@
     <t>Tên đội</t>
   </si>
   <si>
-    <t>Alpha</t>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>DTT</t>
+  </si>
+  <si>
+    <t>best team from ThaiTun</t>
   </si>
   <si>
     <t>Tên thành viên</t>
@@ -56,44 +63,44 @@
     <t>Email</t>
   </si>
   <si>
-    <t>team_manager</t>
-  </si>
-  <si>
     <t>Trưởng đoàn</t>
   </si>
   <si>
-    <t>team_manager@test.com</t>
-  </si>
-  <si>
-    <t>coach</t>
+    <t>coach192</t>
   </si>
   <si>
     <t>Huấn luyện viên</t>
   </si>
   <si>
-    <t>coach@test.com</t>
-  </si>
-  <si>
-    <t>athlete</t>
+    <t>coach192@smashhub.com</t>
+  </si>
+  <si>
+    <t>athlete290</t>
   </si>
   <si>
     <t>Vận động viên</t>
   </si>
   <si>
-    <t>athlete@test.com</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user1@test.com</t>
+    <t>athlete290@smashhub.com</t>
+  </si>
+  <si>
+    <t>athlete291</t>
+  </si>
+  <si>
+    <t>athlete291@smashhub.com</t>
+  </si>
+  <si>
+    <t>team_manager001</t>
+  </si>
+  <si>
+    <t>team_manager001@smashhub.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +115,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,9 +144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -448,16 +462,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBAAF54-F525-44EF-8F60-F6A55BC2E0B8}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5357DB9-DC3D-4751-9CC0-3900478D90A6}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.8984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.69921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -470,13 +524,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,16 +538,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -518,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -535,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>

</xml_diff>